<commit_message>
Synchronize with master branch + Fix display problem + Update component libraries
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Report Generator\git\trunk\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Report Generator\git-repgen\trunk\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -322,9 +322,6 @@
     <t>For instance,  you can choose the number of lines you want to display and you can decide for which Business Criteria, you want to link your placeholder</t>
   </si>
   <si>
-    <t>For more information, please refer to "3- Excel-components-library-info.docx"</t>
-  </si>
-  <si>
     <t>2.23. - Report Generator Version</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>RepGen:TEXT;REPGEN_VERSION</t>
+  </si>
+  <si>
+    <t>For more information, please refer to the official documentation in http://doc.castsoftware.com</t>
   </si>
 </sst>
 </file>
@@ -554,23 +554,23 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,8 +972,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
@@ -984,16 +984,16 @@
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="3"/>
       <c r="E3" s="9"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="3"/>
       <c r="E4" s="9"/>
       <c r="F4" s="1"/>
@@ -1036,31 +1036,31 @@
       <c r="O11" s="2"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="23" t="s">
-        <v>96</v>
+      <c r="C13" s="28" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="13"/>
@@ -1554,12 +1554,12 @@
     </row>
     <row r="113" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B113" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1635,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update templates with doc for VIOLATION_SUMMARY block
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Report Generator\git-repgen\trunk\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMA\AppData\Local\CAST\ReportGenerator\1.3.0\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
     <sheet name="2 - Text blocks" sheetId="8" r:id="rId2"/>
     <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId3"/>
     <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
+    <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -332,6 +333,69 @@
   </si>
   <si>
     <t>For more information, please refer to the official documentation in http://doc.castsoftware.com</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;VIOLATION_SUMMARY;MODULES=1,CRITICAL=1,NONCRITICAL=0,GRADE=1,FAILED=1,ADDEDREMOVED=1,TOTAL=1,SUCCESSFUL=1,COMPLIANCE=1</t>
+  </si>
+  <si>
+    <t>* Block Name = VIOLATION_SUMMARY</t>
+  </si>
+  <si>
+    <t>* Options : MODULE=1|0</t>
+  </si>
+  <si>
+    <t>* Options : CRITICAL=1|0</t>
+  </si>
+  <si>
+    <t>* Options : NONCRITICAL=1|0</t>
+  </si>
+  <si>
+    <t>* Options : GRADE=1|0</t>
+  </si>
+  <si>
+    <t>* Options : TOTAL=1|0</t>
+  </si>
+  <si>
+    <t>* Options : FAILED=1|0</t>
+  </si>
+  <si>
+    <t>* Options : SUCCESSFUL=1|0</t>
+  </si>
+  <si>
+    <t>* Options : ADDEDREMOVED=1|0</t>
+  </si>
+  <si>
+    <t>* Options : COMPLIANCE=1|0</t>
+  </si>
+  <si>
+    <t>display results for application (=0 by default) or per module (=1)</t>
+  </si>
+  <si>
+    <t>include (=1 by default)/do not include (=0) critical violations</t>
+  </si>
+  <si>
+    <t>include (=1)/do not include (=0 by default) non-critical violations</t>
+  </si>
+  <si>
+    <t>show (=1 by default)/hide (=0) "Grade" column</t>
+  </si>
+  <si>
+    <t>show (=1 by default)/hide (=0) "Total Checks" column</t>
+  </si>
+  <si>
+    <t>show (=1)/hide (=0 by default) "# Violations" column</t>
+  </si>
+  <si>
+    <t>show (=1)/hide (=0 by default) "Grade" column</t>
+  </si>
+  <si>
+    <t>show (=1)/hide (=0 by default) "Added" and "Removed" columns</t>
+  </si>
+  <si>
+    <t>show (=1)/hide (=0 by default) "Compliance Ratio" column</t>
+  </si>
+  <si>
+    <t>3.3. - VIOLATION SUMMARY</t>
   </si>
 </sst>
 </file>
@@ -554,6 +618,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -568,9 +635,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -947,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -972,8 +1036,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
@@ -984,16 +1048,16 @@
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="3"/>
       <c r="E3" s="9"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="3"/>
       <c r="E4" s="9"/>
       <c r="F4" s="1"/>
@@ -1036,31 +1100,31 @@
       <c r="O11" s="2"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="23" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="13"/>
@@ -1087,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B116"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
@@ -1636,7 +1700,7 @@
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,4 +1773,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-82 : New "Violation Summary" Table as generic component
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMA\AppData\Local\CAST\ReportGenerator\1.3.0\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="123">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -335,9 +335,6 @@
     <t>For more information, please refer to the official documentation in http://doc.castsoftware.com</t>
   </si>
   <si>
-    <t>RepGen:TABLE;VIOLATION_SUMMARY;MODULES=1,CRITICAL=1,NONCRITICAL=0,GRADE=1,FAILED=1,ADDEDREMOVED=1,TOTAL=1,SUCCESSFUL=1,COMPLIANCE=1</t>
-  </si>
-  <si>
     <t>* Block Name = VIOLATION_SUMMARY</t>
   </si>
   <si>
@@ -386,9 +383,6 @@
     <t>show (=1)/hide (=0 by default) "# Violations" column</t>
   </si>
   <si>
-    <t>show (=1)/hide (=0 by default) "Grade" column</t>
-  </si>
-  <si>
     <t>show (=1)/hide (=0 by default) "Added" and "Removed" columns</t>
   </si>
   <si>
@@ -396,6 +390,18 @@
   </si>
   <si>
     <t>3.3. - VIOLATION SUMMARY</t>
+  </si>
+  <si>
+    <t>show (=1)/hide (=0 by default) "Successful checks" column</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;VIOLATION_SUMMARY;MODULES=0,CRITICAL=1,NONCRITICAL=0,GRADE=1,FAILED=1,ADDEDREMOVED=1,TOTAL=1,SUCCESSFUL=1,COMPLIANCE=1,COUNT=-1</t>
+  </si>
+  <si>
+    <t>* Options : COUNT=-1</t>
+  </si>
+  <si>
+    <t>number of results limited or -1 = all results</t>
   </si>
 </sst>
 </file>
@@ -1777,10 +1783,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C12"/>
+  <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,89 +1796,97 @@
   <sheetData>
     <row r="1" spans="2:3" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>100</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-40 : Update the word, ppt and excel templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="142">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -402,6 +402,63 @@
   </si>
   <si>
     <t>Display only N results or all results if -1 (5 by default)</t>
+  </si>
+  <si>
+    <t>2.24. - Custom Expression</t>
+  </si>
+  <si>
+    <t>* Block Name = CUSTOM_EXPRESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Options = </t>
+  </si>
+  <si>
+    <t>- PARAMS=SZ a SZ b, (SZ pour sizing measure, QR pour quality rule, BF for background fact)</t>
+  </si>
+  <si>
+    <t>- EXPR=b/a, (operators can be +, -, *, / , (, ) )</t>
+  </si>
+  <si>
+    <t>- a=67011,</t>
+  </si>
+  <si>
+    <t>- b=67010,</t>
+  </si>
+  <si>
+    <t>- FORMAT=N0 (N2 by default, if nothing or erroneous format is set),</t>
+  </si>
+  <si>
+    <t>- SNAPSHOT = CURRENT|PREVIOUS with CURRENT by default (or if erroneous or nothing is set) to get the custom expression for the current snapshot or the previous one</t>
+  </si>
+  <si>
+    <t>you could have as number of parameters as you want (theorical limit is 16383 !!)</t>
+  </si>
+  <si>
+    <t>cf https://msdn.microsoft.com/en-us/library/dwhawy9k.aspx for the format</t>
+  </si>
+  <si>
+    <t>(examples for double https://msdn.microsoft.com/en-us/library/kfsatb94.aspx)</t>
+  </si>
+  <si>
+    <t>only N format is interesting here :</t>
+  </si>
+  <si>
+    <t>N: -195,489,100.84</t>
+  </si>
+  <si>
+    <t>N0: -195,489,101</t>
+  </si>
+  <si>
+    <t>N1: -195,489,100.8</t>
+  </si>
+  <si>
+    <t>N2: -195,489,100.84</t>
+  </si>
+  <si>
+    <t>N3: -195,489,100.838</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;CUSTOM_EXPRESSION;PARAMS=SZ a SZ b,EXPR = a/b,a=67011, b=67211,FORMAT=N0</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B116"/>
+  <dimension ref="B2:B136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,8 +1699,104 @@
         <v>98</v>
       </c>
     </row>
+    <row r="118" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B118" s="21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1785,7 +1938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
REPORTGEN-40 : update templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -458,7 +458,7 @@
     <t>N3: -195,489,100.838</t>
   </si>
   <si>
-    <t>RepGen:TEXT;CUSTOM_EXPRESSION;PARAMS=SZ a SZ b,EXPR = a/b,a=67011, b=67211,FORMAT=N0</t>
+    <t>RepGen:TEXT;CUSTOM_EXPRESSION;PARAMS=SZ a SZ b,EXPR = a/b,a=67010, b=67011,FORMAT=N0</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
   <dimension ref="B2:B136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
REPORTGEN-40 : fix templates issues
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="140">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -431,18 +431,6 @@
     <t>- SNAPSHOT = CURRENT|PREVIOUS with CURRENT by default (or if erroneous or nothing is set) to get the custom expression for the current snapshot or the previous one</t>
   </si>
   <si>
-    <t>you could have as number of parameters as you want (theorical limit is 16383 !!)</t>
-  </si>
-  <si>
-    <t>cf https://msdn.microsoft.com/en-us/library/dwhawy9k.aspx for the format</t>
-  </si>
-  <si>
-    <t>(examples for double https://msdn.microsoft.com/en-us/library/kfsatb94.aspx)</t>
-  </si>
-  <si>
-    <t>only N format is interesting here :</t>
-  </si>
-  <si>
     <t>N: -195,489,100.84</t>
   </si>
   <si>
@@ -455,10 +443,16 @@
     <t>N2: -195,489,100.84</t>
   </si>
   <si>
-    <t>N3: -195,489,100.838</t>
-  </si>
-  <si>
-    <t>RepGen:TEXT;CUSTOM_EXPRESSION;PARAMS=SZ a SZ b,EXPR = a/b,a=67010, b=67011,FORMAT=N0</t>
+    <t>You can have as number of parameters as you want (theorical limit is 16383…).</t>
+  </si>
+  <si>
+    <t>The format of return value is explained here : https://msdn.microsoft.com/en-us/library/dwhawy9k.aspx, with examples for double here : https://msdn.microsoft.com/en-us/library/kfsatb94.aspx ), only N format is interesting here :</t>
+  </si>
+  <si>
+    <t>/!\ don’t put blank char in the definition of parameters (,a=67011,b=67010,c=…)</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;CUSTOM_EXPRESSION;PARAMS=SZ a SZ b,EXPR=a/b,a=67010,b=67011,FORMAT=N2</t>
   </si>
 </sst>
 </file>
@@ -468,7 +462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +561,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -631,7 +631,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -698,6 +698,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1212,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B136"/>
+  <dimension ref="B2:B134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,54 +1747,44 @@
         <v>131</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="20" t="s">
+    <row r="127" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B127" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B128" s="29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B129" s="29" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="20" t="s">
+    <row r="130" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B130" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="20" t="s">
+    <row r="131" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B131" s="29" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="20" t="s">
+    <row r="132" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B132" s="29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="20" t="s">
+    <row r="133" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B133" s="29" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="20" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="20" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="20" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-7 : RULE_TOTAL_CHECKS, RULE_FAILED_CHECKS, RULE_FAILED_ON_TOTAL_CHECKS and templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="148">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -145,25 +145,10 @@
     <t>* Block Name = RULE_TOTAL_CHECKS</t>
   </si>
   <si>
-    <t>* Options = RULID=N (by default RULID=7164) where N indicates the rule Id</t>
-  </si>
-  <si>
-    <t>RepGen:TEXT;RULE_TOTAL_CHECKS</t>
-  </si>
-  <si>
     <t>* Block Name = RULE_FAILED_CHECKS</t>
   </si>
   <si>
-    <t>* Options = RULID=N (by default RULID=7126) where N indicates the rule Id</t>
-  </si>
-  <si>
-    <t>RepGen:TEXT;RULE_FAILED_CHECKS</t>
-  </si>
-  <si>
     <t>* Block Name = RULE_FAILED_ON_TOTAL_CHECKS</t>
-  </si>
-  <si>
-    <t>RepGen:TEXT;RULE_FAILED_ON_TOTAL_CHECKS</t>
   </si>
   <si>
     <t>* Block Name = METRIC_EFP_ADDED</t>
@@ -477,6 +462,21 @@
   </si>
   <si>
     <t>RepGen:TEXT;APPLICATION_METRIC;SZID=10151,SNAPSHOT=PREVIOUS,FORMAT=N0</t>
+  </si>
+  <si>
+    <t>- RULID=quality rule id</t>
+  </si>
+  <si>
+    <t>- SNAPSHOT=CURRENT |PREVIOUS (CURRENT by default)</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;RULE_FAILED_ON_TOTAL_CHECKS;RULID=7126,SNAPSHOT=CURRENT</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;RULE_FAILED_CHECKS;RULID=7126</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;RULE_TOTAL_CHECKS;RULID=7126,SNAPSHOT=PREVIOUS</t>
   </si>
 </sst>
 </file>
@@ -1185,14 +1185,14 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
@@ -1240,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B146"/>
+  <dimension ref="B2:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1264,7 @@
   <sheetData>
     <row r="2" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
     </row>
     <row r="7" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
@@ -1299,7 +1299,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
     </row>
     <row r="13" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
@@ -1329,7 +1329,7 @@
     </row>
     <row r="18" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
     </row>
     <row r="23" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
@@ -1369,7 +1369,7 @@
     </row>
     <row r="28" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
@@ -1389,7 +1389,7 @@
     </row>
     <row r="33" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -1409,7 +1409,7 @@
     </row>
     <row r="38" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
     </row>
     <row r="43" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="21" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
@@ -1449,7 +1449,7 @@
     </row>
     <row r="48" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -1469,7 +1469,7 @@
     </row>
     <row r="53" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B53" s="21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
@@ -1489,7 +1489,7 @@
     </row>
     <row r="58" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B58" s="21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
@@ -1499,72 +1499,72 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="20" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="25" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="25" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="20" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B65" s="21" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="20" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="20" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="25" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="25" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="25" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="25" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="20" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B75" s="21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
     </row>
     <row r="80" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B80" s="21" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
     </row>
     <row r="85" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B85" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
@@ -1624,7 +1624,7 @@
     </row>
     <row r="90" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B90" s="21" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
@@ -1634,237 +1634,267 @@
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="20" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B95" s="21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="20" t="s">
-        <v>40</v>
+      <c r="B93" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B97" s="21" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B100" s="21" t="s">
-        <v>135</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="20" t="s">
-        <v>42</v>
+      <c r="B101" s="25" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B105" s="21" t="s">
-        <v>136</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B104" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="20" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="20" t="s">
-        <v>31</v>
+      <c r="B107" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B110" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="20" t="s">
-        <v>46</v>
+      <c r="B108" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B111" s="21" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="20" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B115" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="20" t="s">
-        <v>48</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B116" s="21" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="20" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B120" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="20" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B121" s="21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="20" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B125" s="21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="20" t="s">
-        <v>84</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B126" s="21" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="20" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B130" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="20" t="s">
-        <v>110</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B131" s="21" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="20" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" s="20" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="20" t="s">
-        <v>115</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B136" s="21" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="20" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B139" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B140" s="24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B141" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B142" s="24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B143" s="24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B144" s="24" t="s">
-        <v>121</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="20" t="s">
-        <v>125</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B146" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B147" s="24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B148" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B149" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B150" s="24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B151" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1885,41 +1915,41 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1954,41 +1984,41 @@
   <sheetData>
     <row r="1" spans="2:11" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -2022,97 +2052,97 @@
   <sheetData>
     <row r="1" spans="2:3" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-140 : add component in templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId3"/>
     <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
     <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
+    <sheet name="3-TableBlock-TableMetricIdCol" sheetId="12" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="159">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -477,6 +478,39 @@
   </si>
   <si>
     <t>RepGen:TEXT;RULE_TOTAL_CHECKS;RULID=7126,SNAPSHOT=PREVIOUS</t>
+  </si>
+  <si>
+    <t>3.4. - TABLE_METRIC_ID_COL</t>
+  </si>
+  <si>
+    <t>* Block Name = TABLE_METRIC_ID_COL</t>
+  </si>
+  <si>
+    <t>* Options :</t>
+  </si>
+  <si>
+    <t>- QID : list of Quality indicators (BC or TC or RULE) separated by |</t>
+  </si>
+  <si>
+    <t>- SID : list of Sizing measures separated by |</t>
+  </si>
+  <si>
+    <t>- BID : list of Background facts separated by |</t>
+  </si>
+  <si>
+    <t>- LEVEL : can be APPLICATION or MODULES or TECHNOLOGIES (by default APPLICATION if option not present)</t>
+  </si>
+  <si>
+    <t>- VARIATION = VALUE or PERCENT or BOTH (PERCENT by default)</t>
+  </si>
+  <si>
+    <t>- SNAPSHOT=CURRENT (only CURRENT SNAPSHOT) or PREVIOUS (only PREVIOUS SNAPSHOT) or BOTH (CURRENT and PREVIOUS SNAPSHOT, default option)</t>
+  </si>
+  <si>
+    <t>- HEADER=SHORT, SHORT name is taken if exists, name otherwise</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TABLE_METRIC_ID_COL;QID=60017|60014,SID=10151|67010,BID=66061,LEVEL=APPLICATION,SNAPSHOT=BOTH,VARIATION=BOTH,HEADER=SHORT</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
@@ -2042,7 +2076,7 @@
   <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B1" sqref="B1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,4 +2182,78 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-141 : templates for TABLE_METRIC_ID_ROW
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
     <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
     <sheet name="3-TableBlock-TableMetricIdCol" sheetId="12" r:id="rId6"/>
+    <sheet name="3-TableBlock-TableMetricIdRow" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="162">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -511,6 +512,15 @@
   </si>
   <si>
     <t>RepGen:TABLE;TABLE_METRIC_ID_COL;QID=60017|60014,SID=10151|67010,BID=66061,LEVEL=APPLICATION,SNAPSHOT=BOTH,VARIATION=BOTH,HEADER=SHORT</t>
+  </si>
+  <si>
+    <t>3.5. - TABLE_METRIC_ID_ROW</t>
+  </si>
+  <si>
+    <t>* Block Name = TABLE_METRIC_ID_ROW</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TABLE_METRIC_ID_ROW;QID=60017|60014,SID=10151|67010,BID=66061,LEVEL=APPLICATION,SNAPSHOT=BOTH,VARIATION=BOTH,HEADER=SHORT</t>
   </si>
 </sst>
 </file>
@@ -2188,6 +2198,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B12"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B12"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
@@ -2196,12 +2280,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2249,7 +2333,7 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-152 : update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
     <sheet name="3-TableBlock-TableMetricIdCol" sheetId="12" r:id="rId6"/>
     <sheet name="3-TableBlock-TableMetricIdRow" sheetId="13" r:id="rId7"/>
+    <sheet name="3-TableBlock-TableViolations" sheetId="14" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="167">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -508,9 +509,6 @@
     <t>- SNAPSHOT=CURRENT (only CURRENT SNAPSHOT) or PREVIOUS (only PREVIOUS SNAPSHOT) or BOTH (CURRENT and PREVIOUS SNAPSHOT, default option)</t>
   </si>
   <si>
-    <t>- HEADER=SHORT, SHORT name is taken if exists, name otherwise</t>
-  </si>
-  <si>
     <t>RepGen:TABLE;TABLE_METRIC_ID_COL;QID=60017|60014,SID=10151|67010,BID=66061,LEVEL=APPLICATION,SNAPSHOT=BOTH,VARIATION=BOTH,HEADER=SHORT</t>
   </si>
   <si>
@@ -521,6 +519,24 @@
   </si>
   <si>
     <t>RepGen:TABLE;TABLE_METRIC_ID_ROW;QID=60017|60014,SID=10151|67010,BID=66061,LEVEL=APPLICATION,SNAPSHOT=BOTH,VARIATION=BOTH,HEADER=SHORT</t>
+  </si>
+  <si>
+    <t>* Block Name = TABLE_VIOLATIONS</t>
+  </si>
+  <si>
+    <t>- ID : list of Quality indicators (BC or TC or RULE) separated by |</t>
+  </si>
+  <si>
+    <t>- HEADER=true/1 or false/0, short name is taken if true and exists, name otherwise (default)</t>
+  </si>
+  <si>
+    <t>- CRITICAL=true/1 or false/0 (true by default critical violations are counted, otherwise all violations</t>
+  </si>
+  <si>
+    <t>- DELTA=true/1 or false/0 (true by default, display the added and removed values, otherwise not)</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TABLE_VIOLATIONS;ID=60014|61024|7156,LEVEL=APPLICATION,SNAPSHOT=BOTH,CRITICAL=1, DELTA =1</t>
   </si>
 </sst>
 </file>
@@ -2199,7 +2215,7 @@
   <dimension ref="B1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,7 +2267,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2259,7 +2275,7 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2272,20 +2288,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2325,7 +2341,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2333,7 +2349,76 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bad component name in xl template
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="168">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>RepGen:TABLE;TABLE_VIOLATIONS;ID=60014|61024|7156,LEVEL=APPLICATION,SNAPSHOT=BOTH,CRITICAL=1, DELTA =1</t>
+  </si>
+  <si>
+    <t>3.6. - TABLE_VIOLATIONS</t>
   </si>
 </sst>
 </file>
@@ -2363,14 +2366,14 @@
   <dimension ref="B1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
REPORTGEN-140, REPORTGEN-141 & REPORTGEN-152 : remove components
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -17,9 +17,6 @@
     <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId3"/>
     <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
     <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
-    <sheet name="3-TableBlock-TableMetricIdCol" sheetId="12" r:id="rId6"/>
-    <sheet name="3-TableBlock-TableMetricIdRow" sheetId="13" r:id="rId7"/>
-    <sheet name="3-TableBlock-TableViolations" sheetId="14" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -35,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="148">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -480,72 +477,12 @@
   </si>
   <si>
     <t>RepGen:TEXT;RULE_TOTAL_CHECKS;RULID=7126,SNAPSHOT=PREVIOUS</t>
-  </si>
-  <si>
-    <t>3.4. - TABLE_METRIC_ID_COL</t>
-  </si>
-  <si>
-    <t>* Block Name = TABLE_METRIC_ID_COL</t>
-  </si>
-  <si>
-    <t>* Options :</t>
-  </si>
-  <si>
-    <t>- QID : list of Quality indicators (BC or TC or RULE) separated by |</t>
-  </si>
-  <si>
-    <t>- SID : list of Sizing measures separated by |</t>
-  </si>
-  <si>
-    <t>- BID : list of Background facts separated by |</t>
-  </si>
-  <si>
-    <t>- LEVEL : can be APPLICATION or MODULES or TECHNOLOGIES (by default APPLICATION if option not present)</t>
-  </si>
-  <si>
-    <t>- VARIATION = VALUE or PERCENT or BOTH (PERCENT by default)</t>
-  </si>
-  <si>
-    <t>- SNAPSHOT=CURRENT (only CURRENT SNAPSHOT) or PREVIOUS (only PREVIOUS SNAPSHOT) or BOTH (CURRENT and PREVIOUS SNAPSHOT, default option)</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TABLE_METRIC_ID_COL;QID=60017|60014,SID=10151|67010,BID=66061,LEVEL=APPLICATION,SNAPSHOT=BOTH,VARIATION=BOTH,HEADER=SHORT</t>
-  </si>
-  <si>
-    <t>3.5. - TABLE_METRIC_ID_ROW</t>
-  </si>
-  <si>
-    <t>* Block Name = TABLE_METRIC_ID_ROW</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TABLE_METRIC_ID_ROW;QID=60017|60014,SID=10151|67010,BID=66061,LEVEL=APPLICATION,SNAPSHOT=BOTH,VARIATION=BOTH,HEADER=SHORT</t>
-  </si>
-  <si>
-    <t>* Block Name = TABLE_VIOLATIONS</t>
-  </si>
-  <si>
-    <t>- ID : list of Quality indicators (BC or TC or RULE) separated by |</t>
-  </si>
-  <si>
-    <t>- HEADER=true/1 or false/0, short name is taken if true and exists, name otherwise (default)</t>
-  </si>
-  <si>
-    <t>- CRITICAL=true/1 or false/0 (true by default critical violations are counted, otherwise all violations</t>
-  </si>
-  <si>
-    <t>- DELTA=true/1 or false/0 (true by default, display the added and removed values, otherwise not)</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TABLE_VIOLATIONS;ID=60014|61024|7156,LEVEL=APPLICATION,SNAPSHOT=BOTH,CRITICAL=1, DELTA =1</t>
-  </si>
-  <si>
-    <t>3.6. - TABLE_VIOLATIONS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
@@ -842,7 +779,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90"/>
+        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2104,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,221 +2154,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-247 : Add list of violations for a rule
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId3"/>
     <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
     <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
+    <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="158">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -477,6 +478,36 @@
   </si>
   <si>
     <t>RepGen:TEXT;RULE_TOTAL_CHECKS;RULID=7126,SNAPSHOT=PREVIOUS</t>
+  </si>
+  <si>
+    <t>3.4. - List of violations for a rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Block Name = QUALITY_RULE_VIOLATIONS </t>
+  </si>
+  <si>
+    <t>If Previous snapshot is selected, but there is no previous snapshot, the results from the current snapshot will be displayed.</t>
+  </si>
+  <si>
+    <t>If there is no previous snapshot, column Status is not displayed</t>
+  </si>
+  <si>
+    <t>* BCID= The Id of the business criterion. If this id correspond to efficiency (60014), robustness (60013), or security (60016), the propagatedRiskIndex is displayed. By default, BCID = 60013</t>
+  </si>
+  <si>
+    <t>* ID= The Id of the quality rule for which you want to display the list of violations</t>
+  </si>
+  <si>
+    <t>* COUNT=N where N indicates the top N number ; default value = 10</t>
+  </si>
+  <si>
+    <t>* NAME=FULL|SHORT to display short name or full name of objects (full name by default)</t>
+  </si>
+  <si>
+    <t>* SNAPSHOT=CURRENT|PREVIOUS to select from which snapshot we take results; default is Current</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_RULE_VIOLATIONS;BCID=60013,ID=7424,COUNT=50</t>
   </si>
 </sst>
 </file>
@@ -486,7 +517,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,6 +622,21 @@
       <name val="Corbel"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -655,7 +701,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -727,6 +773,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -2047,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,4 +2202,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-247 : add name of the rule in header and no results when previous and  no snapshot
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -484,9 +484,6 @@
   </si>
   <si>
     <t xml:space="preserve">* Block Name = QUALITY_RULE_VIOLATIONS </t>
-  </si>
-  <si>
-    <t>If Previous snapshot is selected, but there is no previous snapshot, the results from the current snapshot will be displayed.</t>
   </si>
   <si>
     <t>If there is no previous snapshot, column Status is not displayed</t>
@@ -758,6 +755,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -773,8 +772,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1181,8 +1178,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
@@ -1193,16 +1190,16 @@
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="3"/>
       <c r="E3" s="9"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="3"/>
       <c r="E4" s="9"/>
       <c r="F4" s="1"/>
@@ -1250,26 +1247,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="13"/>
@@ -2209,7 +2206,7 @@
   <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,50 +2229,48 @@
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
-        <v>152</v>
+      <c r="B3" s="27" t="s">
+        <v>151</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
-        <v>153</v>
+      <c r="B4" s="27" t="s">
+        <v>152</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
-        <v>154</v>
+      <c r="B5" s="27" t="s">
+        <v>153</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
-        <v>155</v>
+      <c r="B6" s="27" t="s">
+        <v>154</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="32" t="s">
-        <v>156</v>
+      <c r="B7" s="27" t="s">
+        <v>155</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
-        <v>150</v>
-      </c>
+      <c r="B8" s="26"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
     </row>
     <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
-        <v>151</v>
+      <c r="B9" s="26" t="s">
+        <v>150</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -2287,7 +2282,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>

</xml_diff>

<commit_message>
REPORTGEN-45 : Get list of violations for action plan
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
     <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
     <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId6"/>
+    <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -505,12 +506,27 @@
   </si>
   <si>
     <t>RepGen:TABLE;QUALITY_RULE_VIOLATIONS;BCID=60013,ID=7424,COUNT=50</t>
+  </si>
+  <si>
+    <t>3.4. - List of violations in action plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Block Name = ACTION_PLAN_VIOLATIONS </t>
+  </si>
+  <si>
+    <t>* COUNT=N|ALL where N indicates the top N number ; default value = 10 (ALL for all violations)</t>
+  </si>
+  <si>
+    <t>* FILTER=ADDED|SOLVED|PENDING|ALL to filter the list by the violation status; default is ALL</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;ACTION_PLAN_VIOLATIONS;COUNT=10,NAME=SHORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
@@ -775,7 +791,7 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
-    <cellStyle name="Header 1" xfId="1"/>
+    <cellStyle name="Header 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
@@ -1150,7 +1166,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -1290,7 +1306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B152"/>
   <sheetViews>
     <sheetView topLeftCell="A72" workbookViewId="0">
@@ -1955,7 +1971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2009,7 +2025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2089,7 +2105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2202,8 +2218,105 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
+  <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -2216,62 +2329,57 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
-        <v>154</v>
-      </c>
+      <c r="B6" s="26"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
     </row>
-    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
-        <v>155</v>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>161</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
     </row>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="20"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
     </row>
-    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
-        <v>150</v>
-      </c>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
     </row>
@@ -2279,18 +2387,6 @@
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REPORTGEN-282 : Get list of critical violations regarding Business criteria
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
     <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId6"/>
     <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId7"/>
+    <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="167">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -521,6 +522,21 @@
   </si>
   <si>
     <t>RepGen:TABLE;ACTION_PLAN_VIOLATIONS;COUNT=10,NAME=SHORT</t>
+  </si>
+  <si>
+    <t>3.5. - List of critical violations</t>
+  </si>
+  <si>
+    <t>* Block Name = CRITICAL_VIOLATIONS_LIST</t>
+  </si>
+  <si>
+    <t>* BCID=ID1|ID2, by default 60016</t>
+  </si>
+  <si>
+    <t>* FILTER=ADDED|UNCHANGED|ALL to filter the list by the violation status; default is ALL</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;CRITICAL_VIOLATIONS_LIST;BCID=60016,COUNT=ALL</t>
   </si>
 </sst>
 </file>
@@ -2318,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
   <dimension ref="B1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,4 +2408,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
+  <dimension ref="B1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-282 Get list of violations regarding Business criteria
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="169">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -524,19 +524,25 @@
     <t>RepGen:TABLE;ACTION_PLAN_VIOLATIONS;COUNT=10,NAME=SHORT</t>
   </si>
   <si>
-    <t>3.5. - List of critical violations</t>
-  </si>
-  <si>
-    <t>* Block Name = CRITICAL_VIOLATIONS_LIST</t>
-  </si>
-  <si>
     <t>* BCID=ID1|ID2, by default 60016</t>
   </si>
   <si>
-    <t>* FILTER=ADDED|UNCHANGED|ALL to filter the list by the violation status; default is ALL</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;CRITICAL_VIOLATIONS_LIST;BCID=60016,COUNT=ALL</t>
+    <t>3.5. - List of violations by BC</t>
+  </si>
+  <si>
+    <t>* Block Name = VIOLATIONS_LIST</t>
+  </si>
+  <si>
+    <t>* VIOLATIONS=CRITICAL|ALL by default, only CRITICAL violations are listed</t>
+  </si>
+  <si>
+    <t>* MODULE=ModuleName, parameter used to restrict the list for one module, by default violation are listed for the application</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;VIOLATIONS_LIST;BCID=60016,COUNT=ALL</t>
+  </si>
+  <si>
+    <t>* FILTER=ADDED|UNCHANGED|UPDATED|ALL to filter the list by the violation status; default is ALL</t>
   </si>
 </sst>
 </file>
@@ -2412,10 +2418,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
-  <dimension ref="B1:B8"/>
+  <dimension ref="B1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,17 +2431,17 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2450,12 +2456,22 @@
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-282 : add filter by techno
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -30,12 +30,12 @@
     <definedName name="TABLE_4" comment="TEXT;LAST_SNAPSHOT_DATE" localSheetId="0">'1 - Information'!$D$4:$D$4</definedName>
     <definedName name="TABLE_5" comment="TEXT;TODAY_DATE" localSheetId="0">'1 - Information'!$F$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="170">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>* FILTER=ADDED|UNCHANGED|UPDATED|ALL to filter the list by the violation status; default is ALL</t>
+  </si>
+  <si>
+    <t>* TECHNOLOGIES=techno1|techno2, parameter used to restrict the list of violations, by default all TECHNOLOGIES</t>
   </si>
 </sst>
 </file>
@@ -2418,10 +2421,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
-  <dimension ref="B1:B10"/>
+  <dimension ref="B1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,8 +2472,13 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
REPORTGEN-318 : fix bugs from TGU
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -494,9 +494,6 @@
     <t>* BCID= The Id of the business criterion. If this id correspond to efficiency (60014), robustness (60013), or security (60016), the propagatedRiskIndex is displayed. By default, BCID = 60013</t>
   </si>
   <si>
-    <t>* ID= The Id of the quality rule for which you want to display the list of violations</t>
-  </si>
-  <si>
     <t>* COUNT=N where N indicates the top N number ; default value = 10</t>
   </si>
   <si>
@@ -524,9 +521,6 @@
     <t>RepGen:TABLE;ACTION_PLAN_VIOLATIONS;COUNT=10,NAME=SHORT</t>
   </si>
   <si>
-    <t>* BCID=ID1|ID2, by default 60016</t>
-  </si>
-  <si>
     <t>3.5. - List of violations by BC</t>
   </si>
   <si>
@@ -546,6 +540,12 @@
   </si>
   <si>
     <t>* TECHNOLOGIES=techno1|techno2, parameter used to restrict the list of violations, by default all TECHNOLOGIES</t>
+  </si>
+  <si>
+    <t>* BCID= the IDs of Business Criterion separated by | : ID1|ID2, by default 60016</t>
+  </si>
+  <si>
+    <t>* ID= The Id of the quality rule for which you want to display the list of violations, By default, ID = 7788 (Avoid empty catch block)</t>
   </si>
 </sst>
 </file>
@@ -2246,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,28 +2278,28 @@
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -2354,35 +2354,35 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -2423,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
   <dimension ref="B1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,52 +2434,52 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-318 : fix typo
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -496,9 +496,6 @@
     <t>* SNAPSHOT=CURRENT|PREVIOUS to select from which snapshot we take results; default is Current</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_RULE_VIOLATIONS;BCID=60013,ID=7424,COUNT=50</t>
-  </si>
-  <si>
     <t>3.4. - List of violations in action plan</t>
   </si>
   <si>
@@ -551,10 +548,13 @@
     <t>* Note : This component is only relevant on an engineering database. It is not relevant on an analytics database.</t>
   </si>
   <si>
-    <t>Its options and behavior are the same that APPLICATION_METRIC text block</t>
+    <t>This text block has been replaced by the following APPLICATION_METRIC, it has been kept for backward compatibility.</t>
   </si>
   <si>
-    <t>This text block has been replaced by the following APPLICATION_METRIC, it has been kept for backward compatibility.</t>
+    <t>RepGen:TABLE;QUALITY_RULE_VIOLATIONS;BCID=60013,ID=7788,COUNT=50</t>
+  </si>
+  <si>
+    <t>Its options and behavior are the same than APPLICATION_METRIC text block</t>
   </si>
 </sst>
 </file>
@@ -1343,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -1600,12 +1600,12 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2110,7 +2110,7 @@
     <row r="6" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:11" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2254,7 @@
   <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -2368,21 +2368,21 @@
   <sheetData>
     <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -18789,7 +18789,7 @@
     </row>
     <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -18801,7 +18801,7 @@
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -18841,22 +18841,22 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -18866,32 +18866,32 @@
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-420 : update library templates with new component
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8CCFF3-7484-4391-A346-7B0ABFE1D6BD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -20,6 +21,7 @@
     <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId6"/>
     <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId7"/>
     <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId8"/>
+    <sheet name="3 - List of violations statist " sheetId="15" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="183">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -496,9 +498,6 @@
     <t>* SNAPSHOT=CURRENT|PREVIOUS to select from which snapshot we take results; default is Current</t>
   </si>
   <si>
-    <t>3.4. - List of violations in action plan</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Block Name = ACTION_PLAN_VIOLATIONS </t>
   </si>
   <si>
@@ -509,9 +508,6 @@
   </si>
   <si>
     <t>RepGen:TABLE;ACTION_PLAN_VIOLATIONS;COUNT=10,NAME=SHORT</t>
-  </si>
-  <si>
-    <t>3.5. - List of violations by BC</t>
   </si>
   <si>
     <t>* Block Name = VIOLATIONS_LIST</t>
@@ -555,6 +551,42 @@
   </si>
   <si>
     <t>Its options and behavior are the same than APPLICATION_METRIC text block</t>
+  </si>
+  <si>
+    <t>3.5. - List of violations in action plan</t>
+  </si>
+  <si>
+    <t>3.6. - List of violations by BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7. - List of violations statistics by BC, TC or Standard Quality Tag   </t>
+  </si>
+  <si>
+    <t>* Block Name = RULES_LIST_STATISTICS_RATIO</t>
+  </si>
+  <si>
+    <t>* METRICS=List of metrics id (BC, TC or QR) or quality standards tags separated by ‘|’.</t>
+  </si>
+  <si>
+    <t>* CRITICAL=true : add this option if you have selected a BC or a TC and want only critical rules to be selected (by default it is false). This option has no effect on selection by QR or quality standard tag.</t>
+  </si>
+  <si>
+    <t>* COMPLIANCE=true : add this option if you want to display the compliance score column ; by default this column is not displayed.</t>
+  </si>
+  <si>
+    <t>* SORTED=COMPLIANCE : add this option if you want to sort the data by compliance score, from worse to better ; by default the sort of data is from the max number of total violations to the min.</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>To use the quality standard tags selection, the Quality Standards Mapping extension should be installed on the central where the application resides.</t>
+  </si>
+  <si>
+    <t>When you select the metric id for a BC or TC, all the QRs belonging to this BC or TC is added for displaying violations</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=CISQ-Security,COMPLIANCE=true</t>
   </si>
 </sst>
 </file>
@@ -1343,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
@@ -1400,7 +1432,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1472,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -1600,12 +1632,12 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="2:2" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2110,7 +2142,7 @@
     <row r="6" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:11" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="2:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2285,7 +2317,7 @@
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -2325,7 +2357,7 @@
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -2337,7 +2369,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -2358,7 +2390,7 @@
   <dimension ref="A1:XFD12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2368,21 +2400,21 @@
   <sheetData>
     <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -2396,7 +2428,7 @@
     </row>
     <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -18789,7 +18821,7 @@
     </row>
     <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -18801,7 +18833,7 @@
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -18831,7 +18863,7 @@
   <dimension ref="B1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18841,22 +18873,22 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -18866,35 +18898,110 @@
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
+  <dimension ref="B1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27"/>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-411 : new component QUALITY_STANDARDS_EVOLUTION
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8CCFF3-7484-4391-A346-7B0ABFE1D6BD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3731CF7-8571-42AA-84EA-3F82230AC999}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId7"/>
     <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId8"/>
     <sheet name="3 - List of violations statist " sheetId="15" r:id="rId9"/>
+    <sheet name="3 - Evolution of standards" sheetId="16" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="188">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -587,6 +588,21 @@
   </si>
   <si>
     <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=CISQ-Security,COMPLIANCE=true</t>
+  </si>
+  <si>
+    <t>3.8.	Evolution of sub-standards for a quality standard</t>
+  </si>
+  <si>
+    <t>* Block Name = QUALITY_STANDARDS_EVOLUTION</t>
+  </si>
+  <si>
+    <t>* STD= Name of the parent quality standard you want the details, for example, CWE-2011-Top25 will list total, added and removed violations for standards CWE-22, CWE-78, CWE-79, CWE-89, CWE-134, CWE-327, CWE-434 and CWE-798.</t>
+  </si>
+  <si>
+    <t>To use this component, the Quality Standards Mapping extension should be installed on the central where the application resides, with minimum version 20181030</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CWE-2011-Top25</t>
   </si>
 </sst>
 </file>
@@ -1368,6 +1384,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
+  <dimension ref="B1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="27"/>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27"/>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18935,7 +19009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
   <dimension ref="B1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
REPORTGEN-455 : New component for Top Components by properties
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3731CF7-8571-42AA-84EA-3F82230AC999}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D92EF52-8572-4A18-A858-B70FA80040C3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" tabRatio="701" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId8"/>
     <sheet name="3 - List of violations statist " sheetId="15" r:id="rId9"/>
     <sheet name="3 - Evolution of standards" sheetId="16" r:id="rId10"/>
+    <sheet name="3 - Top Components" sheetId="18" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="199">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -603,6 +604,39 @@
   </si>
   <si>
     <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CWE-2011-Top25</t>
+  </si>
+  <si>
+    <t>3.9.	Top components by properties</t>
+  </si>
+  <si>
+    <t>* Block Name = TOP_COMPONENTS_BY_PROPERTIES</t>
+  </si>
+  <si>
+    <t>PROP1 : name of first property, cyclomaticComplexity if not exists</t>
+  </si>
+  <si>
+    <t>PROP2 : name of second property, fanOut if not exists</t>
+  </si>
+  <si>
+    <t>ORDER1 : ASC or DESC for PROP1, DESC by default</t>
+  </si>
+  <si>
+    <t>ORDER2 : ASC or DESC for PROP2, DESC by default</t>
+  </si>
+  <si>
+    <t>COUNT: the number of lines to display, 50 by default (-1 or all is not allowed, it will take too much time and paper)</t>
+  </si>
+  <si>
+    <t>* Options :</t>
+  </si>
+  <si>
+    <t>For PROP1 and PROP2, the available values are : codeLines, commentedCodeLines, commentLines, coupling, fanIn, fanOut, cyclomaticComplexity, ratioCommentLinesCodeLines, halsteadProgramLength, halsteadProgramVocabulary, halsteadVolume, distinctOperators, distinctOperands, integrationComplexity, essentialComplexity</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TOP_COMPONENTS_BY_PROPERTIES;PROP1=cyclomaticComplexity,PROP2=ratioCommentLinesCodeLines,ORDER1=desc,ORDER2=asc,COUNT=10</t>
+  </si>
+  <si>
+    <t>If PROP1 and/or PROP2 is not correctly set,list of available values is displayed</t>
   </si>
 </sst>
 </file>
@@ -1391,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
   <dimension ref="B1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,6 +1471,88 @@
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A48014B-133C-4EB1-BCC8-C47F0FE2BA42}">
+  <dimension ref="B1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-454 : new component RULES_LIST_LARGEST_VARIATION
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D92EF52-8572-4A18-A858-B70FA80040C3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0004CEB-D33A-4408-8063-6BA27E383881}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" tabRatio="701" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="3 - List of violations statist " sheetId="15" r:id="rId9"/>
     <sheet name="3 - Evolution of standards" sheetId="16" r:id="rId10"/>
     <sheet name="3 - Top Components" sheetId="18" r:id="rId11"/>
+    <sheet name="3 - Rules with largest variatio" sheetId="19" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="206">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -637,6 +638,27 @@
   </si>
   <si>
     <t>If PROP1 and/or PROP2 is not correctly set,list of available values is displayed</t>
+  </si>
+  <si>
+    <t>3.10.	List of rules with largest variation</t>
+  </si>
+  <si>
+    <t>* Block Name = RULES_LIST_LARGEST_VARIATION</t>
+  </si>
+  <si>
+    <t>BCID : name of the BCID to get the rule’s compounded weight</t>
+  </si>
+  <si>
+    <t>VARIATION : increase or decrease (decrease by default)</t>
+  </si>
+  <si>
+    <t>DATA : number or percent (number by default)</t>
+  </si>
+  <si>
+    <t>COUNT: the number of lines to display, 50 by default (-1 for all rules)</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_LARGEST_VARIATION;BCID=60011,VARIATION=decrease,DATA=number,COUNT=50</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1483,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A48014B-133C-4EB1-BCC8-C47F0FE2BA42}">
   <dimension ref="B1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1553,6 +1575,69 @@
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321A33B9-4108-40C7-AB52-19B5A9656C7B}">
+  <dimension ref="B1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-482 : headers for RULES_LIST_STATISTICS_RATIO and QUALITY_STANDARD_EVOLUTION should be either Violations, either Vulnerabilities
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0004CEB-D33A-4408-8063-6BA27E383881}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C09B9FB-F22C-446C-AAFE-6282293E958F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" tabRatio="701" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="207">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -589,9 +589,6 @@
     <t>When you select the metric id for a BC or TC, all the QRs belonging to this BC or TC is added for displaying violations</t>
   </si>
   <si>
-    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=CISQ-Security,COMPLIANCE=true</t>
-  </si>
-  <si>
     <t>3.8.	Evolution of sub-standards for a quality standard</t>
   </si>
   <si>
@@ -659,6 +656,12 @@
   </si>
   <si>
     <t>RepGen:TABLE;RULES_LIST_LARGEST_VARIATION;BCID=60011,VARIATION=decrease,DATA=number,COUNT=50</t>
+  </si>
+  <si>
+    <t>*  LBL=violations or vulnerabilities (vulnerabilities if not set), this change the headers from Vulnerabilities to Violations</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=CISQ-Security,COMPLIANCE=true,LBL=violations</t>
   </si>
 </sst>
 </file>
@@ -668,7 +671,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -788,6 +791,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -852,7 +861,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -911,6 +920,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1307,7 +1319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1332,8 +1344,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
@@ -1344,16 +1356,16 @@
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="3"/>
       <c r="E3" s="9"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="3"/>
       <c r="E4" s="9"/>
       <c r="F4" s="1"/>
@@ -1401,26 +1413,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="13"/>
@@ -1445,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:B9"/>
+  <dimension ref="B1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,41 +1470,46 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
+      <c r="B4" s="27" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
-        <v>179</v>
-      </c>
+      <c r="B5" s="27"/>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="27"/>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1516,42 +1533,42 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1559,12 +1576,12 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
@@ -1574,7 +1591,7 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1599,37 +1616,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1637,7 +1654,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -19208,10 +19225,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
-  <dimension ref="B1:B12"/>
+  <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19219,60 +19236,66 @@
     <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="28"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="27"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>182</v>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-79 : update templates and fix issue when no data
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66175D33-6E5D-4C1A-8FBD-1E15426046AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D105629A-EADB-4AA7-9343-49F0A00D86BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995" tabRatio="701" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="3 - Top Components" sheetId="18" r:id="rId11"/>
     <sheet name="3 - Rules with largest variatio" sheetId="19" r:id="rId12"/>
     <sheet name="3 - Removed violations" sheetId="20" r:id="rId13"/>
+    <sheet name="3 - AEFP list" sheetId="22" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="217">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -675,6 +676,24 @@
   </si>
   <si>
     <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50</t>
+  </si>
+  <si>
+    <t>3.12.	List of AEFP</t>
+  </si>
+  <si>
+    <t>* Block Name = AEFP_LIST</t>
+  </si>
+  <si>
+    <t>TYPE : type of the function to display, DF for data function, TF for transactions, by default both are listed</t>
+  </si>
+  <si>
+    <t>STATUS : status of the function to display, ADDED, MODIFIED or DELETED, all statuses by default</t>
+  </si>
+  <si>
+    <t>COUNT: the number of lines to display, 10 by default (-1 for all rules)</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;AEFP_LIST;COUNT=-1</t>
   </si>
 </sst>
 </file>
@@ -684,7 +703,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,6 +829,12 @@
       <name val="Corbel"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -874,7 +899,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -950,6 +975,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1680,7 +1708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53E83-8DB2-4C9D-B684-50883B392432}">
   <dimension ref="B1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1725,6 +1753,72 @@
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6911279-FAB1-4631-AA51-7D78BAFCA198}">
+  <dimension ref="B1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="27"/>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REPORTGEN-508 : update templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0362390B-8BB3-4089-A80E-226EA0E48FB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F598EA-3F6F-4115-B76B-AC4CB71E0447}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="15435" tabRatio="701" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="3 - Removed violations" sheetId="20" r:id="rId13"/>
     <sheet name="3 - components by status list" sheetId="22" r:id="rId14"/>
     <sheet name="3 - AEFP list" sheetId="23" r:id="rId15"/>
+    <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="234">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -884,6 +885,15 @@
   </si>
   <si>
     <t>RepGen:TABLE;DELTA_COMPONENTS_LIST_BY_STATUS;STATUS=deleted,COUNT=-1</t>
+  </si>
+  <si>
+    <t>3.14.	List of AETP</t>
+  </si>
+  <si>
+    <t>* Block Name = AETP_LIST</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;AETP_LIST;COUNT=-1</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6911279-FAB1-4631-AA51-7D78BAFCA198}">
   <dimension ref="B1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2106,6 +2116,62 @@
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822C81FE-2BA1-4A3C-ADB8-F42B4B1305BA}">
+  <dimension ref="B1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REPORTGEN-566 : update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F598EA-3F6F-4115-B76B-AC4CB71E0447}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5C7FC2-4A79-4683-9486-884760C4552F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="15435" tabRatio="701" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="701" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -675,9 +675,6 @@
   </si>
   <si>
     <t>BCID : name of the BCID to get the rule’s compounded weight and to filter results (60017 by default)</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50</t>
   </si>
   <si>
     <t>* Block Name = AEFP_LIST</t>
@@ -895,6 +892,27 @@
   <si>
     <t>RepGen:TABLE;AETP_LIST;COUNT=-1</t>
   </si>
+  <si>
+    <t>UPDATED</t>
+  </si>
+  <si>
+    <r>
+      <t>CRITICITY =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> c for only critical violations, nc for only non critical violations, all for critical and non critical violations (all by default if not configured)</t>
+    </r>
+  </si>
+  <si>
+    <t>RepGen:TABLE;REMOVED_VIOLATIONS_LIST;BCID=60017,COUNT=50,CRITICITY=all</t>
+  </si>
 </sst>
 </file>
 
@@ -903,7 +921,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1042,6 +1060,21 @@
       <name val="Corbel"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1106,7 +1139,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1180,6 +1213,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1905,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53E83-8DB2-4C9D-B684-50883B392432}">
-  <dimension ref="B1:B8"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,41 +1952,49 @@
     <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="I1" s="31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1975,12 +2018,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -1990,37 +2033,37 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2028,27 +2071,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2073,12 +2116,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2088,17 +2131,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -2111,7 +2154,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2127,7 +2170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822C81FE-2BA1-4A3C-ADB8-F42B4B1305BA}">
   <dimension ref="B1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2139,12 +2182,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2154,7 +2197,7 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -2167,7 +2210,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
REPORTGEN-639 : adapt display for only one category and update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBCEFA2-66DB-4C0B-B10C-885CA1E09283}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E70D8F0-14A2-40FE-AC72-786AFF4B77EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="3 - AEFP list" sheetId="23" r:id="rId15"/>
     <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
     <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
+    <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="247">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -891,9 +892,6 @@
     <t>RepGen:TABLE;AETP_LIST;COUNT=-1</t>
   </si>
   <si>
-    <t>UPDATED</t>
-  </si>
-  <si>
     <r>
       <t>CRITICITY =</t>
     </r>
@@ -957,6 +955,18 @@
   </si>
   <si>
     <t>3.15.	Evolution of CAST rules associated to a quality standard category</t>
+  </si>
+  <si>
+    <t>* Block Name = LIST_TAGS_DOC_BYCAT</t>
+  </si>
+  <si>
+    <t>* CAT = Id of the standard quality category, for example, STIG-V4R8-CAT1, or a list separated by ‘|’</t>
+  </si>
+  <si>
+    <t>To use this component, the Quality Standards Mapping extension should be installed on the central where the application resides, with minimum version 20190909</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_TAGS_DOC_BYCAT;CAT=STIG-V4R8-CAT1</t>
   </si>
 </sst>
 </file>
@@ -1275,6 +1285,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1290,7 +1301,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -1695,8 +1705,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1707,16 +1717,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1764,26 +1774,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1811,7 +1821,7 @@
   <dimension ref="B1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,11 +1831,9 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>232</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -1839,12 +1847,12 @@
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2040,9 +2048,7 @@
       <c r="B1" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>232</v>
-      </c>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
@@ -2066,7 +2072,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2074,7 +2080,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2310,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
   <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,25 +2327,23 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>238</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2352,7 +2356,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2363,12 +2367,76 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A93F7-09DE-4CB9-9DC0-106F29CE8F69}">
+  <dimension ref="B1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
REPORTGEN-657: add options for the size of the set and update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\dev\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E70D8F0-14A2-40FE-AC72-786AFF4B77EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FCE157-BDB5-4046-9B71-9490A4D28ECE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="253">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -632,9 +632,6 @@
   </si>
   <si>
     <t>For PROP1 and PROP2, the available values are : codeLines, commentedCodeLines, commentLines, coupling, fanIn, fanOut, cyclomaticComplexity, ratioCommentLinesCodeLines, halsteadProgramLength, halsteadProgramVocabulary, halsteadVolume, distinctOperators, distinctOperands, integrationComplexity, essentialComplexity</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TOP_COMPONENTS_BY_PROPERTIES;PROP1=cyclomaticComplexity,PROP2=ratioCommentLinesCodeLines,ORDER1=desc,ORDER2=asc,COUNT=10</t>
   </si>
   <si>
     <t>If PROP1 and/or PROP2 is not correctly set,list of available values is displayed</t>
@@ -968,6 +965,27 @@
   <si>
     <t>RepGen:TABLE;LIST_TAGS_DOC_BYCAT;CAT=STIG-V4R8-CAT1</t>
   </si>
+  <si>
+    <t>LOWER1 : components should have prop1 value lower than this value</t>
+  </si>
+  <si>
+    <t>GREATER1 : components should have prop1 value greater than this value</t>
+  </si>
+  <si>
+    <t>LOWER2 : components should have prop2 value lower than this value</t>
+  </si>
+  <si>
+    <t>GREATER2 : components should have prop2 value greater than this value</t>
+  </si>
+  <si>
+    <t>UPDATED</t>
+  </si>
+  <si>
+    <t>When using LOWER and GREATER parameters, the ORDER parameter can be overridden to get the most accurate components corresponding to the request. As the filter can be done only after requesting data from the RestAPI, the list can be truncated. So the option NBSET define the number of objects returns from the rest api before the filtering and the limitation of display (COUNT), this option is set to 500 by default, to avoid too long server response time.</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TOP_COMPONENTS_BY_PROPERTIES;PROP1=cyclomaticComplexity,PROP2=ratioCommentLinesCodeLines,ORDER1=desc,ORDER2=asc,LOWER2=0.10,COUNT=100,NBSET=10000</t>
+  </si>
 </sst>
 </file>
 
@@ -976,7 +994,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,6 +1177,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1223,7 +1249,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1286,6 +1312,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1300,6 +1327,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1705,8 +1735,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1717,16 +1747,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1774,26 +1804,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1831,7 +1861,7 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C1" s="26"/>
     </row>
@@ -1847,12 +1877,12 @@
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1887,78 +1917,112 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A48014B-133C-4EB1-BCC8-C47F0FE2BA42}">
-  <dimension ref="B1:B15"/>
+  <dimension ref="B1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="36" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="36" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1983,12 +2047,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -1998,22 +2062,22 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2021,7 +2085,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2046,13 +2110,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2062,17 +2126,17 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2080,7 +2144,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2108,12 +2172,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2123,37 +2187,37 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2161,27 +2225,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2206,12 +2270,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2221,17 +2285,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -2244,7 +2308,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2272,12 +2336,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2351,7 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -2300,7 +2364,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2327,23 +2391,23 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2356,7 +2420,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2367,7 +2431,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2380,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A93F7-09DE-4CB9-9DC0-106F29CE8F69}">
   <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,22 +2454,22 @@
     <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>237</v>
+        <v>241</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2421,7 +2485,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2432,7 +2496,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -20042,7 +20106,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" s="24"/>
     </row>
@@ -20069,7 +20133,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>